<commit_message>
Initial version of version 2.0.0.
</commit_message>
<xml_diff>
--- a/information.xlsx
+++ b/information.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swvanderlaan/git/swvanderlaan/A_primer_in_Human_Cardiovascular_Genetics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slaan3/git/swvanderlaan/A_Practical_Primer_in_Human_Complex_Genetics/background/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82079164-BDD1-9A4E-A12E-55582B230292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8C2A1C-46B3-FD4A-8BB0-351A3F42E375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="22020" windowHeight="14880" activeTab="2" xr2:uid="{B69FCFD0-6F50-0E48-BAC8-87E7AE1C662D}"/>
+    <workbookView xWindow="4320" yWindow="5740" windowWidth="22020" windowHeight="14880" activeTab="1" xr2:uid="{B69FCFD0-6F50-0E48-BAC8-87E7AE1C662D}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs" sheetId="1" r:id="rId1"/>
     <sheet name="Relatedness" sheetId="2" r:id="rId2"/>
     <sheet name="PheWAS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>PLINK</t>
   </si>
@@ -175,6 +176,27 @@
   </si>
   <si>
     <t>1,403 GWAS UK Biobank based</t>
+  </si>
+  <si>
+    <t>IBD0</t>
+  </si>
+  <si>
+    <t>IBD1</t>
+  </si>
+  <si>
+    <t>IBD2</t>
+  </si>
+  <si>
+    <t>Unrelated (includes relationships beyond the third degree)</t>
+  </si>
+  <si>
+    <t>Distantly related</t>
+  </si>
+  <si>
+    <t>&lt;1.56%</t>
+  </si>
+  <si>
+    <t>varies</t>
   </si>
 </sst>
 </file>
@@ -219,9 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -241,9 +264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -387,7 +410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,116 +630,281 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D560C22B-48F0-FC44-AB87-C749B130E0FC}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f>C8+D9</f>
+        <v>0.75</v>
+      </c>
+      <c r="D9">
+        <f>D8/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f>C9+D10</f>
+        <v>0.875</v>
+      </c>
+      <c r="D10">
+        <f>D9/2</f>
+        <v>0.125</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>C10</f>
+        <v>0.875</v>
+      </c>
+      <c r="D11">
+        <f>D10</f>
+        <v>0.125</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f>0.75+0.125+D12</f>
+        <v>0.9375</v>
+      </c>
+      <c r="D12">
+        <f>D11/2</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
+      </c>
+      <c r="C13">
+        <f>C12+D13</f>
+        <v>0.96875</v>
+      </c>
+      <c r="D13">
+        <f>D12/2</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -728,11 +916,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85526057-F8B2-8C4C-B3A4-0ED853A8DE79}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>